<commit_message>
finally done with 11th question
</commit_message>
<xml_diff>
--- a/question11.xlsx
+++ b/question11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashwin\Documents\GitHub\sim-mod-analysis-asst2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB07C9E-9443-44C0-9879-5D761BED0BD8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1DED40-8D51-4D23-94AA-345B6FC231B1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{A5413CED-3C4E-4465-B353-A98AD842B378}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="20">
   <si>
     <t>Interval(Seconds)</t>
   </si>
@@ -88,13 +88,16 @@
   </si>
   <si>
     <t>Random Numbers Generated</t>
+  </si>
+  <si>
+    <t>And solutions for the selceted random numbers in next sheet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,8 +133,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,6 +151,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -168,11 +183,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -188,9 +204,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -503,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCEB2B04-8D6E-4057-8622-ADD29C40AEDC}">
-  <dimension ref="C5:K18"/>
+  <dimension ref="C5:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,7 +579,7 @@
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="G6" s="5">
-        <f xml:space="preserve"> 15/E6</f>
+        <f xml:space="preserve"> 15/F6</f>
         <v>225</v>
       </c>
       <c r="I6" s="2" t="s">
@@ -588,8 +608,8 @@
         <v>0.2</v>
       </c>
       <c r="G7" s="5">
-        <f t="shared" ref="G7:G12" si="1" xml:space="preserve"> 15/E7</f>
-        <v>112.5</v>
+        <f xml:space="preserve"> 15/(F7-F6)</f>
+        <v>112.49999999999997</v>
       </c>
       <c r="I7" s="3">
         <v>12282</v>
@@ -615,12 +635,12 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="F8" s="5">
-        <f t="shared" ref="F8:F12" si="2">E8+F7</f>
+        <f t="shared" ref="F8:F12" si="1">E8+F7</f>
         <v>0.3666666666666667</v>
       </c>
       <c r="G8" s="5">
-        <f t="shared" si="1"/>
-        <v>90</v>
+        <f t="shared" ref="G8:G12" si="2" xml:space="preserve"> 15/(F8-F7)</f>
+        <v>89.999999999999986</v>
       </c>
       <c r="I8" s="3">
         <v>50391</v>
@@ -646,12 +666,12 @@
         <v>0.23333333333333334</v>
       </c>
       <c r="F9" s="5">
+        <f t="shared" si="1"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="G9" s="5">
         <f t="shared" si="2"/>
-        <v>0.60000000000000009</v>
-      </c>
-      <c r="G9" s="5">
-        <f xml:space="preserve"> 15/E9</f>
-        <v>64.285714285714278</v>
+        <v>64.285714285714263</v>
       </c>
       <c r="I9" s="3">
         <v>95878</v>
@@ -677,12 +697,12 @@
         <v>0.2</v>
       </c>
       <c r="F10" s="5">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="G10" s="5">
         <f t="shared" si="2"/>
-        <v>0.8</v>
-      </c>
-      <c r="G10" s="5">
-        <f t="shared" si="1"/>
-        <v>75</v>
+        <v>75.000000000000014</v>
       </c>
       <c r="I10" s="3">
         <v>82697</v>
@@ -708,12 +728,12 @@
         <v>0.13333333333333333</v>
       </c>
       <c r="F11" s="5">
+        <f t="shared" si="1"/>
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="G11" s="5">
         <f t="shared" si="2"/>
-        <v>0.93333333333333335</v>
-      </c>
-      <c r="G11" s="5">
-        <f t="shared" si="1"/>
-        <v>112.5</v>
+        <v>112.50000000000003</v>
       </c>
       <c r="I11" s="3">
         <v>35712</v>
@@ -739,12 +759,12 @@
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="F12" s="5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G12" s="5">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G12" s="5">
-        <f t="shared" si="1"/>
-        <v>225</v>
+        <v>225.00000000000006</v>
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.3">
@@ -755,10 +775,19 @@
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C19" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="I5:K5"/>
     <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -769,7 +798,7 @@
   <dimension ref="C4:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:C10"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -811,51 +840,101 @@
       <c r="C6" s="3">
         <v>50.003700000000002</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="D6" s="3">
+        <v>48.001100000000001</v>
+      </c>
+      <c r="E6" s="3">
+        <v>47.400300000000001</v>
+      </c>
+      <c r="F6" s="3">
+        <v>47.220100000000002</v>
+      </c>
+      <c r="G6" s="3">
+        <v>47.165999999999997</v>
+      </c>
+      <c r="H6" s="3">
+        <v>47.149799999999999</v>
+      </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C7" s="3">
         <v>158.61435000000003</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="D7" s="3">
+        <v>156.97999999999999</v>
+      </c>
+      <c r="E7" s="3">
+        <v>156.36799999999999</v>
+      </c>
+      <c r="F7" s="3">
+        <v>156.13800000000001</v>
+      </c>
+      <c r="G7" s="3">
+        <v>156.05199999999999</v>
+      </c>
+      <c r="H7" s="3">
+        <v>156.01900000000001</v>
+      </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C8" s="3">
         <v>288.25230000000005</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="D8" s="3">
+        <v>200.68799999999999</v>
+      </c>
+      <c r="E8" s="3">
+        <v>193.39099999999999</v>
+      </c>
+      <c r="F8" s="3">
+        <v>192.78299999999999</v>
+      </c>
+      <c r="G8" s="3">
+        <v>192.732</v>
+      </c>
+      <c r="H8" s="3">
+        <v>192.72800000000001</v>
+      </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C9" s="3">
         <v>250.68645000000004</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="D9" s="3">
+        <v>197.55699999999999</v>
+      </c>
+      <c r="E9" s="3">
+        <v>193.13</v>
+      </c>
+      <c r="F9" s="3">
+        <v>192.761</v>
+      </c>
+      <c r="G9" s="3">
+        <v>192.73</v>
+      </c>
+      <c r="H9" s="3">
+        <v>192.72800000000001</v>
+      </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C10" s="3">
         <v>116.77920000000002</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="D10" s="3">
+        <v>106.69499999999999</v>
+      </c>
+      <c r="E10" s="3">
+        <v>104.17400000000001</v>
+      </c>
+      <c r="F10" s="3">
+        <v>103.54300000000001</v>
+      </c>
+      <c r="G10" s="3">
+        <v>103.386</v>
+      </c>
+      <c r="H10" s="3">
+        <v>103.346</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>